<commit_message>
Fix errors and add data example for pyTest
</commit_message>
<xml_diff>
--- a/project/excel/dataset_ap.xlsx
+++ b/project/excel/dataset_ap.xlsx
@@ -7,9 +7,17 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Dataset" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="DatasetCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Thing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Intangible" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CreativeWork" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Dataset" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="DatasetCollection" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="MaterialEntity" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ChemicalEntity" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="ChemicalReaction" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="ReactionStep" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="PlannedProcess" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Assay" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,17 +434,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>identifier</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>url</t>
         </is>
       </c>
     </row>
@@ -445,68 +468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>primary_email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -519,11 +481,702 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>has_input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_output</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>citation</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dateCreated</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>dateModified</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>datePublished</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>hasPart</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>isAccessibleForFree</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>isBasedOn</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>isPartOf</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>maintainer</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>publisher</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AA1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>distribution</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>includedInDataCatalog</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>issn</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>measurementMethod</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>measurementTechnique</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>variableMeasured</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>conformsTo</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>citation</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>dateCreated</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>dateModified</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>datePublished</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>hasPart</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>isAccessibleForFree</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>isBasedOn</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>isPartOf</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>maintainer</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>publisher</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:W1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>datasets</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>measurementMethod</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>measurementTechnique</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>citation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>dateCreated</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dateModified</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>datePublished</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>hasPart</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>isAccessibleForFree</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>isBasedOn</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>isPartOf</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>maintainer</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>publisher</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>url</t>
         </is>
       </c>
     </row>

</xml_diff>